<commit_message>
Completed version with security consideration.
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -20,6 +20,46 @@
     <author>sam</author>
   </authors>
   <commentList>
+    <comment ref="A4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+Password can be stored in plan text or encrypted text. (Plain text is unsafe)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>Encrypted format:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve"> {cipher}eRK+QiKGLHo8vWbARRGKLgMGvh2UKB7afrPnYdiqJKgbCQs5a/yBxRs96rHICvBWTcYJB9/EllIaWPVSLUIU2RIJNwRpwJfDJyetALmhf0JolQAdWCsIMQ78y4Ub2x6SpMhKxDTI9JbfoWxbPI6BDL7crIzcPB/wWZNQEr/xQIdSlCDLFri8/bwZZig7BQuzmpFyF4tcUlJ0pjxE3gSUkXGetvPvT2yy8ze8kzhfcNAu7CTscaHEenIVALRIHvWWn7xeZP+Ap4gBI+AT5p88Klb+UD7E1bB1WB7d/0/+swDZVLmx0Vjf4P41+CEwllzd44Sr4KYZ52emiWDH66Bjiw==</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="A7" authorId="0">
       <text>
         <r>
@@ -47,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34">
   <si>
     <t>Table 1</t>
   </si>
@@ -55,19 +95,19 @@
     <t>JDBC_URL</t>
   </si>
   <si>
-    <t>jdbc:mysql://rm-wz95ai33k1cqdscy21o.mysql.rds.aliyuncs.com:3306/huotuo?useUnicode=true&amp;characterEncoding=UTF-8&amp;useSSL=false</t>
+    <t>jdbc:mysql://localhost:3306/test?useUnicode=true&amp;characterEncoding=UTF-8&amp;useSSL=false</t>
   </si>
   <si>
     <t>USERNAME</t>
   </si>
   <si>
-    <t>tst</t>
+    <t>test</t>
   </si>
   <si>
     <t>PASSWORD</t>
   </si>
   <si>
-    <t>test</t>
+    <t>{cipher}eRK+QiKGLHo8vWbARRGKLgMGvh2UKB7afrPnYdiqJKgbCQs5a/yBxRs96rHICvBWTcYJB9/EllIaWPVSLUIU2RIJNwRpwJfDJyetALmhf0JolQAdWCsIMQ78y4Ub2x6SpMhKxDTI9JbfoWxbPI6BDL7crIzcPB/wWZNQEr/xQIdSlCDLFri8/bwZZig7BQuzmpFyF4tcUlJ0pjxE3gSUkXGetvPvT2yy8ze8kzhfcNAu7CTscaHEenIVALRIHvWWn7xeZP+Ap4gBI+AT5p88Klb+UD7E1bB1WB7d/0/+swDZVLmx0Vjf4P41+CEwllzd44Sr4KYZ52emiWDH66Bjiw==</t>
   </si>
   <si>
     <t>DB_TYPE</t>
@@ -116,6 +156,39 @@
   </si>
   <si>
     <t>If no table_name.sql defined, will use "select * from table_name"</t>
+  </si>
+  <si>
+    <t>For Password</t>
+  </si>
+  <si>
+    <t>Password is strongly recommended to be encrypted</t>
+  </si>
+  <si>
+    <t>E.G. {cipher}eRK+QiKGLHo8vWbARRGKLgMGvh2UKB7afrPnYdiqJKgbCQs5a/yBxRs96rHICvBWTcYJB9/EllIaWPVSLUIU2RIJNwRpwJfDJyetALmhf0JolQAdWCsIMQ78y4Ub2x6SpMhKxDTI9JbfoWxbPI6BDL7crIzcPB/wWZNQEr/xQIdSlCDLFri8/bwZZig7BQuzmpFyF4tcUlJ0pjxE3gSUkXGetvPvT2yy8ze8kzhfcNAu7CTscaHEenIVALRIHvWWn7xeZP+Ap4gBI+AT5p88Klb+UD7E1bB1WB7d/0/+swDZVLmx0Vjf4P41+CEwllzd44Sr4KYZ52emiWDH66Bjiw==</t>
+  </si>
+  <si>
+    <t>Usage:</t>
+  </si>
+  <si>
+    <t>You should deploy in three steps:</t>
+  </si>
+  <si>
+    <t>First time deploy, run init function first. (One-off work on one server)</t>
+  </si>
+  <si>
+    <t>java -jar xxx.jar -init &lt;app_id&gt;</t>
+  </si>
+  <si>
+    <t>Ask your IAM team to encrypt the password for you</t>
+  </si>
+  <si>
+    <t>java -jar xxx.jar -encrypt &lt;your db password&gt;</t>
+  </si>
+  <si>
+    <t>When you got the encrypted password, input to the config.xlsx</t>
+  </si>
+  <si>
+    <t>Run the program</t>
   </si>
 </sst>
 </file>
@@ -124,13 +197,26 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="25">
     <font>
       <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
@@ -158,14 +244,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -173,6 +260,21 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -186,6 +288,68 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Helvetica Neue"/>
@@ -193,11 +357,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -209,98 +372,21 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -309,19 +395,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor indexed="12"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -333,169 +569,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -569,11 +661,56 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -593,17 +730,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -613,47 +746,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -671,171 +763,180 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2016,134 +2117,134 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3303571428571" defaultRowHeight="19.9" customHeight="1" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="21.8660714285714" style="2" customWidth="1"/>
-    <col min="2" max="2" width="162.642857142857" style="2" customWidth="1"/>
-    <col min="3" max="251" width="16.3482142857143" style="2" customWidth="1"/>
+    <col min="1" max="1" width="21.8660714285714" style="5" customWidth="1"/>
+    <col min="2" max="2" width="162.642857142857" style="5" customWidth="1"/>
+    <col min="3" max="251" width="16.3482142857143" style="5" customWidth="1"/>
     <col min="252" max="252" width="16.3482142857143"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1" spans="1:2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="6"/>
     </row>
     <row r="2" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="11" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
     </row>
     <row r="10" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="10"/>
     </row>
     <row r="11" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="10"/>
     </row>
     <row r="12" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="10"/>
     </row>
     <row r="13" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="10"/>
     </row>
     <row r="14" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="10"/>
     </row>
     <row r="15" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="10"/>
     </row>
     <row r="16" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="11"/>
     </row>
     <row r="17" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A17" s="6"/>
-      <c r="B17" s="7"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="10"/>
     </row>
     <row r="18" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A18" s="6"/>
-      <c r="B18" s="7"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="10"/>
     </row>
     <row r="19" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A19" s="6"/>
-      <c r="B19" s="7"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="10"/>
     </row>
     <row r="20" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A20" s="6"/>
-      <c r="B20" s="7"/>
+      <c r="A20" s="9"/>
+      <c r="B20" s="10"/>
     </row>
     <row r="21" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A21" s="6"/>
-      <c r="B21" s="7"/>
+      <c r="A21" s="9"/>
+      <c r="B21" s="10"/>
     </row>
     <row r="22" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A22" s="6"/>
-      <c r="B22" s="7"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2161,58 +2262,127 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A17" sqref="A17:B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.4" outlineLevelRow="6" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="16.8" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="27.0803571428571" customWidth="1"/>
-    <col min="2" max="2" width="13.8303571428571" customWidth="1"/>
-    <col min="3" max="3" width="19.3392857142857" customWidth="1"/>
-    <col min="4" max="4" width="15.1696428571429" customWidth="1"/>
+    <col min="1" max="1" width="27.0803571428571" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.8303571428571" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.3392857142857" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1696428571429" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.14285714285714" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14" customHeight="1" spans="3:3">
-      <c r="C1" t="s">
+    <row r="1" ht="22" customHeight="1" spans="3:3">
+      <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" ht="13" spans="1:3">
-      <c r="A2" t="s">
+    <row r="2" ht="17" spans="1:3">
+      <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" ht="13" spans="2:3">
-      <c r="B3" t="s">
+    <row r="3" ht="17" spans="2:3">
+      <c r="B3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" ht="13" spans="2:3">
-      <c r="B4" t="s">
+    <row r="4" ht="17" spans="2:3">
+      <c r="B4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" ht="13" spans="1:2">
-      <c r="A7" t="s">
+    <row r="7" ht="17" spans="1:2">
+      <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="9" ht="17" spans="1:2">
+      <c r="A9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2">
+      <c r="B10" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" ht="22" customHeight="1" spans="1:2">
+      <c r="A17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" ht="22" customHeight="1" spans="1:2">
+      <c r="A18" s="1">
+        <v>1</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" ht="22" customHeight="1" spans="2:2">
+      <c r="B19" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" ht="22" customHeight="1" spans="1:2">
+      <c r="A20" s="1">
+        <v>2</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" ht="22" customHeight="1" spans="2:2">
+      <c r="B21" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" ht="22" customHeight="1" spans="1:2">
+      <c r="A22" s="1">
+        <v>3</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" ht="22" customHeight="1" spans="1:2">
+      <c r="A23" s="1">
+        <v>4</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" ht="22" customHeight="1" spans="2:2">
+      <c r="B24" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
To support business date, for back-date running purpose.
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -107,7 +107,7 @@
     <t>PASSWORD</t>
   </si>
   <si>
-    <t>{cipher}eRK+QiKGLHo8vWbARRGKLgMGvh2UKB7afrPnYdiqJKgbCQs5a/yBxRs96rHICvBWTcYJB9/EllIaWPVSLUIU2RIJNwRpwJfDJyetALmhf0JolQAdWCsIMQ78y4Ub2x6SpMhKxDTI9JbfoWxbPI6BDL7crIzcPB/wWZNQEr/xQIdSlCDLFri8/bwZZig7BQuzmpFyF4tcUlJ0pjxE3gSUkXGetvPvT2yy8ze8kzhfcNAu7CTscaHEenIVALRIHvWWn7xeZP+Ap4gBI+AT5p88Klb+UD7E1bB1WB7d/0/+swDZVLmx0Vjf4P41+CEwllzd44Sr4KYZ52emiWDH66Bjiw==</t>
+    <t>{cipher}XLD5fMCgmMl7dy3F0tmwsHlsqvVVxO04VOy/TD/bKMYxHhwei020XwASmrL8xnZgPjpXhhV6T/9J6C2CQ2FNBIK0+OYiG1HMVySpVt1tmgZ4AfuDzyuNa3yqSEgNsURK/PBwJzdw6AuOB7VlNmCx4DIjb5l0a4VeUX5ZivJ3dD4qDka2jPJV5GkhusTzMBBfymj8V3SxeHNRL8dHmeBhhQHpQ3AGS94tk/uhEPPN6PBDKXaoVFDQiq1u0olfYT3tV7bucdE0iWj+Gbf0t2nBKwTCworDUUnzjX2CpHGu/qjaEfibNfnmNVcwnzIlvMzEo5QdiiPw3hwJ4M7gHsO7Ug==</t>
   </si>
   <si>
     <t>DB_TYPE</t>
@@ -196,10 +196,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -235,6 +235,73 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -243,40 +310,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C6500"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -288,23 +333,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="3"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
@@ -320,71 +350,41 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -407,187 +407,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -715,6 +715,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -726,17 +737,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -763,148 +763,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2117,7 +2117,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3303571428571" defaultRowHeight="19.9" customHeight="1" outlineLevelCol="1"/>

</xml_diff>

<commit_message>
Update to support password-encryption-web project
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28000" windowHeight="14160"/>
+    <workbookView windowWidth="28000" windowHeight="14760"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <author>sam</author>
   </authors>
   <commentList>
-    <comment ref="A4" authorId="0">
+    <comment ref="A3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -60,7 +60,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0">
+    <comment ref="A6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -87,10 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36">
-  <si>
-    <t>Table 1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35">
   <si>
     <t>JDBC_URL</t>
   </si>
@@ -192,6 +189,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">For back date processing or run in testing environment, you might want to specify </t>
     </r>
     <r>
@@ -213,12 +216,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="26">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -245,12 +248,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <color indexed="8"/>
@@ -258,6 +255,134 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -266,66 +391,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -334,81 +399,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C6500"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="14"/>
       <color rgb="FFFF0000"/>
       <name val="Helvetica Neue"/>
@@ -436,121 +433,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -562,61 +613,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -690,26 +687,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -744,16 +741,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -783,7 +780,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -792,152 +789,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -959,16 +956,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2142,14 +2136,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3303571428571" defaultRowHeight="19.9" customHeight="1" outlineLevelCol="1"/>
@@ -2160,128 +2154,119 @@
     <col min="252" max="252" width="16.3482142857143"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.65" customHeight="1" spans="1:2">
+    <row r="1" ht="20.25" customHeight="1" spans="1:2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-    </row>
-    <row r="2" ht="20.25" customHeight="1" spans="1:2">
-      <c r="A2" s="8" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+    </row>
+    <row r="2" ht="20.05" customHeight="1" spans="1:2">
+      <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
+      <c r="B2" s="10" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A3" s="10" t="s">
-        <v>3</v>
+      <c r="A3" s="9" t="s">
+        <v>4</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A4" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="12" t="s">
+      <c r="A4" s="9" t="s">
         <v>6</v>
       </c>
+      <c r="B4" s="10" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="5" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A5" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="11" t="s">
+      <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
+      <c r="B5" s="10" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A6" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="11" t="s">
+      <c r="A6" s="9" t="s">
         <v>10</v>
       </c>
+      <c r="B6" s="10" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A7" s="10" t="s">
-        <v>11</v>
+      <c r="A7" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A8" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>14</v>
-      </c>
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
     </row>
     <row r="9" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
     </row>
     <row r="10" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="10"/>
     </row>
     <row r="11" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="10"/>
     </row>
     <row r="12" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="10"/>
     </row>
     <row r="13" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A13" s="10"/>
-      <c r="B13" s="11"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="10"/>
     </row>
     <row r="14" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A14" s="10"/>
-      <c r="B14" s="11"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="10"/>
     </row>
     <row r="15" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A15" s="10"/>
+      <c r="A15" s="9"/>
       <c r="B15" s="11"/>
     </row>
     <row r="16" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A16" s="10"/>
-      <c r="B16" s="12"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="10"/>
     </row>
     <row r="17" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="10"/>
     </row>
     <row r="18" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A18" s="10"/>
-      <c r="B18" s="11"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="10"/>
     </row>
     <row r="19" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A19" s="10"/>
-      <c r="B19" s="11"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="10"/>
     </row>
     <row r="20" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A20" s="10"/>
-      <c r="B20" s="11"/>
+      <c r="A20" s="9"/>
+      <c r="B20" s="10"/>
     </row>
     <row r="21" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A21" s="10"/>
-      <c r="B21" s="11"/>
-    </row>
-    <row r="22" ht="20.05" customHeight="1" spans="1:2">
-      <c r="A22" s="10"/>
-      <c r="B22" s="11"/>
+      <c r="A21" s="9"/>
+      <c r="B21" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
-  </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277777777777778" footer="0.277777777777778"/>
   <pageSetup paperSize="1" scale="72" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
@@ -2296,8 +2281,8 @@
   <sheetPr/>
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A4" sqref="$A4:$XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="16.8" outlineLevelCol="2"/>
@@ -2311,63 +2296,63 @@
   <sheetData>
     <row r="1" ht="22" customHeight="1" spans="3:3">
       <c r="C1" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" ht="17" spans="1:3">
       <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" ht="17" spans="2:3">
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" ht="17" spans="2:3">
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" ht="17" spans="1:2">
       <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="9" ht="17" spans="1:2">
       <c r="A9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="10" spans="2:2">
       <c r="B10" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" ht="22" customHeight="1" spans="1:2">
       <c r="A17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="18" ht="22" customHeight="1" spans="1:2">
@@ -2375,12 +2360,12 @@
         <v>1</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" ht="22" customHeight="1" spans="2:2">
       <c r="B19" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" ht="22" customHeight="1" spans="1:2">
@@ -2388,12 +2373,12 @@
         <v>2</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" ht="22" customHeight="1" spans="2:2">
       <c r="B21" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" ht="22" customHeight="1" spans="1:2">
@@ -2401,7 +2386,7 @@
         <v>3</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" ht="22" customHeight="1" spans="1:2">
@@ -2409,12 +2394,12 @@
         <v>4</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" ht="22" customHeight="1" spans="2:2">
       <c r="B24" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" ht="17" spans="1:2">
@@ -2422,12 +2407,12 @@
         <v>5</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="2:2">
       <c r="B26" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>